<commit_message>
height new init guesses
</commit_message>
<xml_diff>
--- a/supplementary/data3/height.xlsx
+++ b/supplementary/data3/height.xlsx
@@ -1183,7 +1183,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1220,13 +1220,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.025676212086857</v>
+        <v>7.045666640060215</v>
       </c>
       <c r="C2" t="n">
-        <v>7.005207675546093</v>
+        <v>7.024070785879318</v>
       </c>
       <c r="D2" t="n">
-        <v>7.046694535660443</v>
+        <v>7.068606660591883</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -1239,13 +1239,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2657817549210068</v>
+        <v>0.2635746963958489</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2515738222741532</v>
+        <v>0.2497931573575791</v>
       </c>
       <c r="D3" t="n">
-        <v>0.279410334832804</v>
+        <v>0.2758344047487104</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -1258,13 +1258,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.09360765303284038</v>
+        <v>0.08857221122974394</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0860061163555491</v>
+        <v>0.0800544941117232</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1015953908548237</v>
+        <v>0.0972025988418975</v>
       </c>
       <c r="E4" t="n">
         <v>0.15</v>
@@ -1273,52 +1273,62 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>SNR</t>
+          <t>pi</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.243704621305181</v>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+        <v>0.1690695024872479</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1550406136442121</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1849592257737052</v>
+      </c>
       <c r="E5" t="n">
-        <v>1.252966351636703</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>MCC</t>
+          <t>Keq</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9556100546852627</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+        <v>0.2045596611001532</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.1834888352933051</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.2269325133359767</v>
+      </c>
       <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Recall</t>
+          <t>SNR</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9665071770334929</v>
+        <v>1.242102391096362</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>1.252966351636703</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Precision</t>
+          <t>MCC</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9596199524940617</v>
+        <v>0.9501101656941288</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -1327,11 +1337,11 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>Recall</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2065</v>
+        <v>0.9665071770334929</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -1340,11 +1350,11 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>Precision</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>17</v>
+        <v>0.9505882352941176</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -1353,11 +1363,11 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>14</v>
+        <v>2061</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -1366,11 +1376,11 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>404</v>
+        <v>21</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -1379,32 +1389,45 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>p(specific)</t>
+          <t>FN</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.9971104911739581</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.9838296970136762</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.9981381792240068</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>pi</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>404</v>
+      </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="n">
-        <v>0.15</v>
-      </c>
+      <c r="E14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>p(specific)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.9971550724362235</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.9829524118352336</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.9982796597731458</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1417,7 +1440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1454,13 +1477,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.005398985677058</v>
+        <v>7.002403255994217</v>
       </c>
       <c r="C2" t="n">
-        <v>6.986706843924773</v>
+        <v>6.981462514546145</v>
       </c>
       <c r="D2" t="n">
-        <v>7.025882512786813</v>
+        <v>7.02464650658167</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -1473,13 +1496,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2161735921165374</v>
+        <v>0.2082011137697973</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2065305238086126</v>
+        <v>0.1980091052580437</v>
       </c>
       <c r="D3" t="n">
-        <v>0.225501462342905</v>
+        <v>0.217351398503064</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -1492,13 +1515,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1577208517393283</v>
+        <v>0.1542698026731528</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1484949816689978</v>
+        <v>0.1433309674317986</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1686415800836434</v>
+        <v>0.1652123308767115</v>
       </c>
       <c r="E4" t="n">
         <v>0.15</v>
@@ -1507,52 +1530,62 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>SNR</t>
+          <t>pi</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3.777836589444367</v>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+        <v>0.172155532464627</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1584130878392987</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1876643266692657</v>
+      </c>
       <c r="E5" t="n">
-        <v>3.75889905491011</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>MCC</t>
+          <t>Keq</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9799840914864164</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+        <v>0.2090268040384629</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.1882314066731731</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.2310182362033923</v>
+      </c>
       <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Recall</t>
+          <t>SNR</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9880382775119617</v>
+        <v>3.787464886780817</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>3.75889905491011</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Precision</t>
+          <t>MCC</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9786729857819905</v>
+        <v>0.9872644337931913</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -1561,11 +1594,11 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>Recall</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2073</v>
+        <v>1</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -1574,11 +1607,11 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>Precision</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>9</v>
+        <v>0.9789227166276346</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -1587,11 +1620,11 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>5</v>
+        <v>2073</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -1600,11 +1633,11 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>413</v>
+        <v>9</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -1613,32 +1646,45 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>p(specific)</t>
+          <t>FN</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.9977434587537986</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.9950877359825548</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.9984371402340294</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>pi</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>418</v>
+      </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="n">
-        <v>0.15</v>
-      </c>
+      <c r="E14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>p(specific)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.9980787137566742</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.9959616337693512</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.9986518429881251</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1651,7 +1697,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1688,13 +1734,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.056622191941567</v>
+        <v>7.07349675139366</v>
       </c>
       <c r="C2" t="n">
-        <v>7.037358256217418</v>
+        <v>7.053463604281482</v>
       </c>
       <c r="D2" t="n">
-        <v>7.076459297217191</v>
+        <v>7.094774165389631</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -1707,13 +1753,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2518163866640079</v>
+        <v>0.2574715802754098</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2331759018780709</v>
+        <v>0.2361045088700503</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2722797191350208</v>
+        <v>0.2766826638105736</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -1726,13 +1772,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.005371359290845851</v>
+        <v>0.005421152423837016</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0036084057720747</v>
+        <v>0.0034900398193405</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0076685571167224</v>
+        <v>0.0076828171014041</v>
       </c>
       <c r="E4" t="n">
         <v>0.15</v>
@@ -1741,52 +1787,62 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>SNR</t>
+          <t>pi</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9875252447750269</v>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+        <v>0.06332600858951332</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.0549945913397197</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.0735408577087472</v>
+      </c>
       <c r="E5" t="n">
-        <v>0.751779810982022</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>MCC</t>
+          <t>Keq</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.5280455509959634</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+        <v>0.06812092695272719</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.0581950066556524</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0793784156590914</v>
+      </c>
       <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Recall</t>
+          <t>SNR</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.3373205741626794</v>
+        <v>0.9904470064400045</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>0.751779810982022</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Precision</t>
+          <t>MCC</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9527027027027027</v>
+        <v>0.5409238290051372</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -1795,11 +1851,11 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>Recall</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2075</v>
+        <v>0.3492822966507177</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -1808,11 +1864,11 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>Precision</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>7</v>
+        <v>0.9605263157894737</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -1821,11 +1877,11 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>277</v>
+        <v>2076</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -1834,11 +1890,11 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>141</v>
+        <v>6</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -1847,32 +1903,45 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>p(specific)</t>
+          <t>FN</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.1965218480688918</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.0158314628309736</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.9299567823516612</v>
-      </c>
+        <v>272</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>pi</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>146</v>
+      </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="n">
-        <v>0.15</v>
-      </c>
+      <c r="E14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>p(specific)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.2217227088717977</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0204550055096</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.9324294690783776</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1885,7 +1954,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1922,13 +1991,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.048128946789306</v>
+        <v>7.059015117397855</v>
       </c>
       <c r="C2" t="n">
-        <v>7.028865284177364</v>
+        <v>7.039819917945227</v>
       </c>
       <c r="D2" t="n">
-        <v>7.065817614621853</v>
+        <v>7.079401315885056</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -1941,13 +2010,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2267001844225698</v>
+        <v>0.2282630600540152</v>
       </c>
       <c r="C3" t="n">
-        <v>0.194755686400854</v>
+        <v>0.1972488121896742</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2567562945860331</v>
+        <v>0.256975395962566</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -1960,13 +2029,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.0004019071914709411</v>
+        <v>0.0003834971905524366</v>
       </c>
       <c r="C4" t="n">
-        <v>4.020996491163e-05</v>
+        <v>3.894641274271258e-05</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0011475307297276</v>
+        <v>0.0010629815662089</v>
       </c>
       <c r="E4" t="n">
         <v>0.15</v>
@@ -1975,52 +2044,62 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>SNR</t>
+          <t>pi</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9816485686770919</v>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+        <v>0.0210501501404922</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.0160529441382324</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.027571007442035</v>
+      </c>
       <c r="E5" t="n">
-        <v>0.6264831758183516</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>MCC</t>
+          <t>Keq</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.2870012001876636</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+        <v>0.02178400975400969</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.0163148457880377</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0283527260774196</v>
+      </c>
       <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Recall</t>
+          <t>SNR</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.1004784688995215</v>
+        <v>0.9820972422119491</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>0.6264831758183516</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Precision</t>
+          <t>MCC</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9767441860465116</v>
+        <v>0.2833926746282168</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -2029,11 +2108,11 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>Recall</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2081</v>
+        <v>0.09808612440191387</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -2042,11 +2121,11 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>Precision</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>0.9761904761904762</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -2055,11 +2134,11 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>376</v>
+        <v>2081</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -2068,11 +2147,11 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -2081,32 +2160,45 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>p(specific)</t>
+          <t>FN</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.01645667002212479</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.0015724529862261</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.2793609441259058</v>
-      </c>
+        <v>377</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>pi</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>41</v>
+      </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="n">
-        <v>0.15</v>
-      </c>
+      <c r="E14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>p(specific)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.01851704329482102</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0024099929981779</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.2771150204350676</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2119,7 +2211,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2156,13 +2248,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.009780722324763</v>
+        <v>7.05060816933291</v>
       </c>
       <c r="C2" t="n">
-        <v>6.990182556270979</v>
+        <v>7.030399428238984</v>
       </c>
       <c r="D2" t="n">
-        <v>7.030289479555247</v>
+        <v>7.072072472317366</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -2175,13 +2267,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2225266529115568</v>
+        <v>0.2236212296332172</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2113839430654761</v>
+        <v>0.2114554443373899</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2331407639197432</v>
+        <v>0.2345035113056477</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -2194,13 +2286,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1543660330450897</v>
+        <v>0.1500845875224803</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1440683999228787</v>
+        <v>0.1397354517934541</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1649036715933091</v>
+        <v>0.1604270580224904</v>
       </c>
       <c r="E4" t="n">
         <v>0.15</v>
@@ -2209,52 +2301,62 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>SNR</t>
+          <t>pi</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2.508773721497945</v>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+        <v>0.1722656679673565</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1578364119390096</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1885811740700711</v>
+      </c>
       <c r="E5" t="n">
-        <v>2.505932703273406</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>MCC</t>
+          <t>Keq</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9785257584601095</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+        <v>0.2092471477166206</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.1874177589312958</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.2324092069311598</v>
+      </c>
       <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Recall</t>
+          <t>SNR</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9856459330143541</v>
+        <v>2.505393026998103</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>2.505932703273406</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Precision</t>
+          <t>MCC</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9786223277909739</v>
+        <v>0.985872538113183</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -2263,11 +2365,11 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>Recall</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2073</v>
+        <v>1</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -2276,11 +2378,11 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>Precision</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>9</v>
+        <v>0.9766355140186916</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -2289,11 +2391,11 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>6</v>
+        <v>2072</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -2302,11 +2404,11 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>412</v>
+        <v>10</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -2315,32 +2417,45 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>p(specific)</t>
+          <t>FN</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.9975454473278392</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.9954145428935228</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.9982441068497164</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>pi</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>418</v>
+      </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="n">
-        <v>0.15</v>
-      </c>
+      <c r="E14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>p(specific)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.9977327515969827</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.9958212406156824</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.9983041892730328</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2353,7 +2468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2390,13 +2505,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.018238555982022</v>
+        <v>7.018242528267781</v>
       </c>
       <c r="C2" t="n">
-        <v>6.997334838358437</v>
+        <v>6.998382017682101</v>
       </c>
       <c r="D2" t="n">
-        <v>7.037540588480795</v>
+        <v>7.039336557429747</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -2409,13 +2524,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9401239410625015</v>
+        <v>0.9856466455816224</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0296735790364519</v>
+        <v>0.0556521706325387</v>
       </c>
       <c r="D3" t="n">
-        <v>2.92307840977131</v>
+        <v>2.803347554338533</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -2428,13 +2543,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.000209535627799779</v>
+        <v>0.0002102811732126914</v>
       </c>
       <c r="C4" t="n">
-        <v>1.477787671511774e-05</v>
+        <v>1.233093848017683e-05</v>
       </c>
       <c r="D4" t="n">
-        <v>0.000672511743281</v>
+        <v>0.000639164227538</v>
       </c>
       <c r="E4" t="n">
         <v>0.15</v>
@@ -2443,46 +2558,56 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>SNR</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+          <t>pi</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.0002232403806305561</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.439330896312842e-07</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.0009427445730553</v>
+      </c>
       <c r="E5" t="n">
-        <v>0.375889905491011</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>MCC</t>
+          <t>Keq</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+        <v>0.0002079606866114075</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1.439331104080949e-07</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0009436341790913</v>
+      </c>
       <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Recall</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
+          <t>SNR</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>0.375889905491011</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Precision</t>
+          <t>MCC</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -2495,11 +2620,11 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>Recall</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2082</v>
+        <v>0</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -2508,7 +2633,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>Precision</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -2521,11 +2646,11 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>418</v>
+        <v>2082</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -2534,7 +2659,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -2547,32 +2672,45 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>p(specific)</t>
+          <t>FN</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>7.149859684658642e-08</v>
-      </c>
-      <c r="C13" t="n">
-        <v>3.298493197758563e-08</v>
-      </c>
-      <c r="D13" t="n">
-        <v>4.054696379903902e-07</v>
-      </c>
+        <v>418</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>pi</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="n">
-        <v>0.15</v>
-      </c>
+      <c r="E14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>p(specific)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>7.217432913670787e-07</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2.962465166711093e-07</v>
+      </c>
+      <c r="D15" t="n">
+        <v>4.42916035634375e-06</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2585,7 +2723,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2622,13 +2760,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.027165299538193</v>
+        <v>7.054000435805193</v>
       </c>
       <c r="C2" t="n">
-        <v>7.006657753583137</v>
+        <v>7.033769391687988</v>
       </c>
       <c r="D2" t="n">
-        <v>7.045225273026229</v>
+        <v>7.07548844784866</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -2641,13 +2779,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2378899059040618</v>
+        <v>0.2339676520336393</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2278911533841347</v>
+        <v>0.2212960258747685</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2487663700725236</v>
+        <v>0.2452796477360611</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -2660,13 +2798,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1420827807964802</v>
+        <v>0.1390502609944779</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1318960490019367</v>
+        <v>0.1291250338947962</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1530561450145302</v>
+        <v>0.1489811956440249</v>
       </c>
       <c r="E4" t="n">
         <v>0.15</v>
@@ -2675,52 +2813,62 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>SNR</t>
+          <t>pi</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.87107196852589</v>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+        <v>0.1729933057917888</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1585443396826645</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1893212095221891</v>
+      </c>
       <c r="E5" t="n">
-        <v>1.879449527455055</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>MCC</t>
+          <t>Keq</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9757934464391493</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+        <v>0.2103131779304319</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.1884167494860625</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.233534224158218</v>
+      </c>
       <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Recall</t>
+          <t>SNR</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9880382775119617</v>
+        <v>1.869605946326443</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>1.879449527455055</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Precision</t>
+          <t>MCC</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.971764705882353</v>
+        <v>0.983102325103148</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -2729,11 +2877,11 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>Recall</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2070</v>
+        <v>1</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -2742,11 +2890,11 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>Precision</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>12</v>
+        <v>0.9720930232558139</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -2755,11 +2903,11 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>5</v>
+        <v>2070</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -2768,11 +2916,11 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>413</v>
+        <v>12</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -2781,32 +2929,45 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>p(specific)</t>
+          <t>FN</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.9975545421452305</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.9958726676041962</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.998139640039187</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>pi</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>418</v>
+      </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="n">
-        <v>0.15</v>
-      </c>
+      <c r="E14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>p(specific)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.9976052459415424</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.996025906405838</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.998141064712272</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2819,7 +2980,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2856,13 +3017,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.07460612591967</v>
+        <v>7.08131422667592</v>
       </c>
       <c r="C2" t="n">
-        <v>7.054983671107198</v>
+        <v>7.059479161137181</v>
       </c>
       <c r="D2" t="n">
-        <v>7.094812846533568</v>
+        <v>7.104508573652176</v>
       </c>
       <c r="E2" t="n">
         <v>7</v>
@@ -2875,13 +3036,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2728767817599605</v>
+        <v>0.2808176552948126</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2580226979444396</v>
+        <v>0.2643298516918523</v>
       </c>
       <c r="D3" t="n">
-        <v>0.288930920246653</v>
+        <v>0.2955005163077077</v>
       </c>
       <c r="E3" t="n">
         <v>0.2</v>
@@ -2894,13 +3055,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.02352064654634942</v>
+        <v>0.02210332882060337</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0196271961407736</v>
+        <v>0.0179392241655186</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0281325748420292</v>
+        <v>0.0265318205229178</v>
       </c>
       <c r="E4" t="n">
         <v>0.15</v>
@@ -2909,52 +3070,62 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>SNR</t>
+          <t>pi</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.035572027087388</v>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+        <v>0.122546670450689</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1104217713404032</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1369158344784649</v>
+      </c>
       <c r="E5" t="n">
-        <v>0.9397247637275276</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>MCC</t>
+          <t>Keq</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.8102152646203993</v>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+        <v>0.1405310414169987</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.1241283165094819</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.1586355543365352</v>
+      </c>
       <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Recall</t>
+          <t>SNR</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.7272727272727273</v>
+        <v>1.037976459463451</v>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>0.9397247637275276</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Precision</t>
+          <t>MCC</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9620253164556962</v>
+        <v>0.8005233604207933</v>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
@@ -2963,11 +3134,11 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>Recall</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2070</v>
+        <v>0.722488038277512</v>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
@@ -2976,11 +3147,11 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>FP</t>
+          <t>Precision</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>12</v>
+        <v>0.949685534591195</v>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
@@ -2989,11 +3160,11 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>114</v>
+        <v>2066</v>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
@@ -3002,11 +3173,11 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>FP</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>304</v>
+        <v>16</v>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
@@ -3015,32 +3186,45 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>p(specific)</t>
+          <t>FN</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.9351287197082763</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.2490678654857967</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.9983719393175304</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>pi</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>302</v>
+      </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="n">
-        <v>0.15</v>
-      </c>
+      <c r="E14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>p(specific)</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.9200204807550827</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.2368953215363656</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.9984809577788616</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>